<commit_message>
huanyi done . some bug fix
</commit_message>
<xml_diff>
--- a/赞助人员列表.xlsx
+++ b/赞助人员列表.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crainax/war3/LH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\War3\Maps\Loopinghell\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27315" windowHeight="13545" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>赞助人员列表</t>
     <rPh sb="0" eb="1">
@@ -198,6 +195,90 @@
     <rPh sb="2" eb="3">
       <t xml:space="preserve"> </t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>丨袖手旁观丨</t>
+  </si>
+  <si>
+    <t>小牛同志丶</t>
+  </si>
+  <si>
+    <t>不武酱</t>
+  </si>
+  <si>
+    <t>蓝瘦香菇mmm</t>
+  </si>
+  <si>
+    <t>以可爱出名#5383</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣灵死法师</t>
+  </si>
+  <si>
+    <t>SAODIH</t>
+  </si>
+  <si>
+    <t>玩腻玛个皮皮蛋</t>
+  </si>
+  <si>
+    <t>玩东方入魔的超#5563</t>
+  </si>
+  <si>
+    <t>猪食</t>
+  </si>
+  <si>
+    <t>小黑爱大白</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>悲欢离合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nickyly129</t>
+  </si>
+  <si>
+    <t>金笙丶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>羁绊轮回</t>
+  </si>
+  <si>
+    <t>相守不离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郝可怜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亲爱的老王叔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>千枫落</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>q856101589</t>
+  </si>
+  <si>
+    <t>XXI1235</t>
+  </si>
+  <si>
+    <t>佛丿大湿兄</t>
+  </si>
+  <si>
+    <t>我是怪叔叔</t>
+  </si>
+  <si>
+    <t>我才不需要</t>
+  </si>
+  <si>
+    <t>play</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -205,7 +286,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -641,20 +722,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F6:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="158" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="158" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" customWidth="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
+    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.875" customWidth="1"/>
+    <col min="11" max="11" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.25" customWidth="1"/>
+    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="6:15" ht="15" thickBot="1"/>
+    <row r="7" spans="6:15">
       <c r="F7" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +753,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="6:15">
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -680,7 +765,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="6:15">
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -692,7 +777,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:15" ht="15" thickBot="1">
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -704,7 +789,7 @@
       <c r="N10" s="8"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="6:15">
       <c r="F11" t="s">
         <v>1</v>
       </c>
@@ -717,8 +802,20 @@
       <c r="I11">
         <v>1386963254</v>
       </c>
-    </row>
-    <row r="12" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11">
+        <v>24682425</v>
+      </c>
+      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11">
+        <v>1199483482</v>
+      </c>
+    </row>
+    <row r="12" spans="6:15">
       <c r="F12" t="s">
         <v>2</v>
       </c>
@@ -731,8 +828,20 @@
       <c r="I12">
         <v>920323633</v>
       </c>
-    </row>
-    <row r="13" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12">
+        <v>838476900</v>
+      </c>
+      <c r="L12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12">
+        <v>85817056</v>
+      </c>
+    </row>
+    <row r="13" spans="6:15">
       <c r="F13" t="s">
         <v>3</v>
       </c>
@@ -745,8 +854,20 @@
       <c r="I13">
         <v>2028760546</v>
       </c>
-    </row>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13">
+        <v>21235704</v>
+      </c>
+      <c r="L13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13">
+        <v>1884797690</v>
+      </c>
+    </row>
+    <row r="14" spans="6:15">
       <c r="F14" t="s">
         <v>4</v>
       </c>
@@ -759,8 +880,20 @@
       <c r="I14">
         <v>76404545</v>
       </c>
-    </row>
-    <row r="15" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14">
+        <v>259338775</v>
+      </c>
+      <c r="L14" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14">
+        <v>138245006</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15">
       <c r="F15" t="s">
         <v>5</v>
       </c>
@@ -773,8 +906,20 @@
       <c r="I15">
         <v>772953595</v>
       </c>
-    </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15">
+        <v>1945313488</v>
+      </c>
+      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15">
+        <v>55883798</v>
+      </c>
+    </row>
+    <row r="16" spans="6:15">
       <c r="F16" t="s">
         <v>9</v>
       </c>
@@ -787,8 +932,20 @@
       <c r="I16">
         <v>122150585</v>
       </c>
-    </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16">
+        <v>185409653</v>
+      </c>
+      <c r="L16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16">
+        <v>237209239</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13">
       <c r="F17" t="s">
         <v>10</v>
       </c>
@@ -801,8 +958,20 @@
       <c r="I17">
         <v>1866394937</v>
       </c>
-    </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17">
+        <v>848895504</v>
+      </c>
+      <c r="L17" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17">
+        <v>208207478</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13">
       <c r="F18" t="s">
         <v>8</v>
       </c>
@@ -815,8 +984,14 @@
       <c r="I18">
         <v>668865994</v>
       </c>
-    </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18">
+        <v>970908405</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13">
       <c r="F19" t="s">
         <v>6</v>
       </c>
@@ -829,8 +1004,14 @@
       <c r="I19">
         <v>11465124</v>
       </c>
-    </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19">
+        <v>1406966725</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13">
       <c r="F20" t="s">
         <v>11</v>
       </c>
@@ -843,40 +1024,94 @@
       <c r="I20">
         <v>1483305270</v>
       </c>
-    </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20">
+        <v>476387019</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13">
       <c r="F21" t="s">
         <v>12</v>
       </c>
       <c r="G21">
         <v>243951516</v>
       </c>
-    </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>2096927165</v>
+      </c>
+      <c r="J21" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21">
+        <v>1407806903</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13">
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22">
         <v>472054031</v>
       </c>
-    </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22">
+        <v>89160614</v>
+      </c>
+      <c r="J22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22">
+        <v>39350822</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13">
       <c r="F23" t="s">
         <v>14</v>
       </c>
       <c r="G23">
         <v>156566316</v>
       </c>
-    </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23">
+        <v>416503868</v>
+      </c>
+      <c r="J23" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23">
+        <v>947015907</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13">
       <c r="F24" t="s">
         <v>15</v>
       </c>
       <c r="G24">
         <v>805389327</v>
       </c>
-    </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24">
+        <v>366425370</v>
+      </c>
+      <c r="J24" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24">
+        <v>1524326451</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13">
       <c r="F27" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
2.68 and B publish!!!!!!!!!!
</commit_message>
<xml_diff>
--- a/赞助人员列表.xlsx
+++ b/赞助人员列表.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>赞助人员列表</t>
     <rPh sb="0" eb="1">
@@ -536,6 +536,67 @@
   </si>
   <si>
     <t>简单灬情</t>
+  </si>
+  <si>
+    <t>王老四</t>
+  </si>
+  <si>
+    <t>欧豪666</t>
+  </si>
+  <si>
+    <t>Biu凯凯</t>
+  </si>
+  <si>
+    <t>DDxZZD</t>
+  </si>
+  <si>
+    <t>莫魂</t>
+  </si>
+  <si>
+    <t>沈卡子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张思四</t>
+  </si>
+  <si>
+    <t>神天道至尊</t>
+  </si>
+  <si>
+    <t>狂吃小笼包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ghj999</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7kss</t>
+  </si>
+  <si>
+    <t>阿迪王上</t>
+  </si>
+  <si>
+    <t>灬Cyf</t>
+  </si>
+  <si>
+    <t>奈奈吖丶</t>
+  </si>
+  <si>
+    <t>丨朽木</t>
+  </si>
+  <si>
+    <t>小V亮1</t>
+  </si>
+  <si>
+    <t>逍-遥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小林先生0</t>
+  </si>
+  <si>
+    <t>哔哔哔哔哔哔丶</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F6:Q49"/>
+  <dimension ref="F6:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H34" zoomScale="158" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43:M45"/>
+    <sheetView tabSelected="1" topLeftCell="I49" zoomScale="158" workbookViewId="0">
+      <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1908,6 +1969,12 @@
       </c>
     </row>
     <row r="47" spans="12:17">
+      <c r="L47" t="s">
+        <v>132</v>
+      </c>
+      <c r="M47">
+        <v>904823142</v>
+      </c>
       <c r="P47" t="s">
         <v>122</v>
       </c>
@@ -1916,6 +1983,12 @@
       </c>
     </row>
     <row r="48" spans="12:17">
+      <c r="L48" t="s">
+        <v>133</v>
+      </c>
+      <c r="M48">
+        <v>13683093</v>
+      </c>
       <c r="P48" t="s">
         <v>123</v>
       </c>
@@ -1923,12 +1996,146 @@
         <v>1088397663</v>
       </c>
     </row>
-    <row r="49" spans="16:17">
+    <row r="49" spans="12:17">
+      <c r="L49" t="s">
+        <v>134</v>
+      </c>
+      <c r="M49">
+        <v>1242297465</v>
+      </c>
       <c r="P49" t="s">
         <v>124</v>
       </c>
       <c r="Q49">
         <v>1193547207</v>
+      </c>
+    </row>
+    <row r="50" spans="12:17">
+      <c r="L50" t="s">
+        <v>135</v>
+      </c>
+      <c r="M50">
+        <v>610812043</v>
+      </c>
+    </row>
+    <row r="51" spans="12:17">
+      <c r="L51" t="s">
+        <v>136</v>
+      </c>
+      <c r="M51">
+        <v>225975698</v>
+      </c>
+    </row>
+    <row r="52" spans="12:17">
+      <c r="L52" t="s">
+        <v>137</v>
+      </c>
+      <c r="M52">
+        <v>1778330124</v>
+      </c>
+    </row>
+    <row r="53" spans="12:17">
+      <c r="L53" t="s">
+        <v>138</v>
+      </c>
+      <c r="M53">
+        <v>1021570043</v>
+      </c>
+    </row>
+    <row r="54" spans="12:17">
+      <c r="L54" t="s">
+        <v>139</v>
+      </c>
+      <c r="M54">
+        <v>22278263</v>
+      </c>
+    </row>
+    <row r="55" spans="12:17">
+      <c r="L55" t="s">
+        <v>140</v>
+      </c>
+      <c r="M55">
+        <v>534339887</v>
+      </c>
+    </row>
+    <row r="56" spans="12:17">
+      <c r="L56" t="s">
+        <v>141</v>
+      </c>
+      <c r="M56">
+        <v>46380924</v>
+      </c>
+    </row>
+    <row r="57" spans="12:17">
+      <c r="L57" t="s">
+        <v>142</v>
+      </c>
+      <c r="M57">
+        <v>434531878</v>
+      </c>
+    </row>
+    <row r="58" spans="12:17">
+      <c r="L58" t="s">
+        <v>143</v>
+      </c>
+      <c r="M58">
+        <v>48827206</v>
+      </c>
+    </row>
+    <row r="59" spans="12:17">
+      <c r="L59" t="s">
+        <v>144</v>
+      </c>
+      <c r="M59">
+        <v>23689807</v>
+      </c>
+    </row>
+    <row r="60" spans="12:17">
+      <c r="L60" t="s">
+        <v>145</v>
+      </c>
+      <c r="M60">
+        <v>601303810</v>
+      </c>
+    </row>
+    <row r="61" spans="12:17">
+      <c r="L61" t="s">
+        <v>146</v>
+      </c>
+      <c r="M61">
+        <v>2024814813</v>
+      </c>
+    </row>
+    <row r="62" spans="12:17">
+      <c r="L62" t="s">
+        <v>147</v>
+      </c>
+      <c r="M62">
+        <v>1965676132</v>
+      </c>
+    </row>
+    <row r="63" spans="12:17">
+      <c r="L63" t="s">
+        <v>148</v>
+      </c>
+      <c r="M63">
+        <v>1356170852</v>
+      </c>
+    </row>
+    <row r="64" spans="12:17">
+      <c r="L64" t="s">
+        <v>149</v>
+      </c>
+      <c r="M64">
+        <v>730864612</v>
+      </c>
+    </row>
+    <row r="65" spans="12:13">
+      <c r="L65" t="s">
+        <v>150</v>
+      </c>
+      <c r="M65">
+        <v>415945636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>